<commit_message>
WIP Bevoegdheden -> Procids
</commit_message>
<xml_diff>
--- a/MDT/Dienstencatalogus.xlsx
+++ b/MDT/Dienstencatalogus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="14352" windowHeight="5700" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="14352" windowHeight="5700" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Bron RDW.nl" sheetId="1" r:id="rId1"/>
@@ -852,10 +852,10 @@
     <t>Aanvragen gewaarmerkt uittrekstel rijvaardigheid</t>
   </si>
   <si>
-    <t>[Bevoegdheid]</t>
-  </si>
-  <si>
-    <t>Bevoegdheid</t>
+    <t>ProcID</t>
+  </si>
+  <si>
+    <t>[ProcID]</t>
   </si>
 </sst>
 </file>
@@ -2152,7 +2152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -2666,9 +2666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2678,7 +2676,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B1" t="s">
         <v>179</v>
@@ -2686,7 +2684,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>

</xml_diff>